<commit_message>
excel parser updated as per new excel sheet.
</commit_message>
<xml_diff>
--- a/RulesApp/src/main/resources/sample/NPV Model Inputs 1.28.2014.xlsx
+++ b/RulesApp/src/main/resources/sample/NPV Model Inputs 1.28.2014.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\e-nirvana\docs\proj-docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\e-nirvana\src-code\3pam\proj-docs\latest\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1186" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1193" uniqueCount="391">
   <si>
     <t>Name</t>
   </si>
@@ -1476,6 +1476,27 @@
   </si>
   <si>
     <t>MonthEnd(CFKPaidDate)-1month+1day</t>
+  </si>
+  <si>
+    <t>DisplayName</t>
+  </si>
+  <si>
+    <t>Motnhly Servicing Fee</t>
+  </si>
+  <si>
+    <t>Format</t>
+  </si>
+  <si>
+    <t>Money</t>
+  </si>
+  <si>
+    <t>DisplayOrder</t>
+  </si>
+  <si>
+    <t>AlwaysRequired</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -1529,7 +1550,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1560,12 +1581,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1589,7 +1604,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1621,19 +1636,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1646,6 +1652,17 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma 2" xfId="1"/>
@@ -1957,10 +1974,10 @@
   <sheetPr codeName="Sheet4">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P145"/>
+  <dimension ref="A1:S145"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1968,12 +1985,18 @@
     <col min="1" max="1" width="19.140625" style="4" customWidth="1"/>
     <col min="2" max="2" width="30.7109375" customWidth="1"/>
     <col min="3" max="3" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="13" width="8.7109375" customWidth="1" outlineLevel="1"/>
-    <col min="14" max="14" width="95.42578125" bestFit="1" customWidth="1" outlineLevel="1"/>
-    <col min="15" max="15" width="18.5703125" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="8.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="13" width="8.7109375" customWidth="1" outlineLevel="1"/>
+    <col min="14" max="14" width="11.42578125" customWidth="1" outlineLevel="1"/>
+    <col min="15" max="15" width="8" customWidth="1" outlineLevel="1"/>
+    <col min="16" max="16" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>153</v>
       </c>
@@ -2019,8 +2042,20 @@
       <c r="O1" s="1" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P1" s="25" t="s">
+        <v>384</v>
+      </c>
+      <c r="Q1" s="25" t="s">
+        <v>386</v>
+      </c>
+      <c r="R1" s="25" t="s">
+        <v>388</v>
+      </c>
+      <c r="S1" s="25" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>154</v>
       </c>
@@ -2066,8 +2101,20 @@
       <c r="O2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P2" t="s">
+        <v>385</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>387</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>16</v>
       </c>
@@ -2111,7 +2158,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
         <v>52</v>
       </c>
@@ -2155,7 +2202,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="10" t="s">
         <v>140</v>
       </c>
@@ -2199,7 +2246,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
         <v>165</v>
       </c>
@@ -2243,10 +2290,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="6"/>
     </row>
-    <row r="8" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>156</v>
       </c>
@@ -2288,7 +2335,7 @@
       </c>
       <c r="N8" s="8"/>
     </row>
-    <row r="9" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>36</v>
       </c>
@@ -2326,7 +2373,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>46</v>
       </c>
@@ -2364,7 +2411,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>56</v>
       </c>
@@ -2405,7 +2452,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>44</v>
       </c>
@@ -2446,7 +2493,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>34</v>
       </c>
@@ -2490,7 +2537,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="9" t="s">
         <v>35</v>
       </c>
@@ -2534,7 +2581,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>38</v>
       </c>
@@ -2575,7 +2622,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:15" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>40</v>
       </c>
@@ -4710,13 +4757,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E102"/>
+  <dimension ref="A1:E103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="A27" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4747,16 +4794,16 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="17" t="s">
         <v>341</v>
       </c>
       <c r="E2" s="6" t="s">
@@ -4764,16 +4811,16 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="18" t="s">
         <v>342</v>
       </c>
       <c r="E3" s="6" t="s">
@@ -4781,100 +4828,100 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="15" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="22" t="s">
         <v>323</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="22" t="s">
         <v>323</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="16" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="22" t="s">
         <v>146</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="22" t="s">
         <v>146</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="16" t="s">
         <v>378</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="22" t="s">
         <v>144</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="22" t="s">
         <v>144</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="16" t="s">
         <v>379</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="22" t="s">
         <v>169</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="22" t="s">
         <v>169</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="16" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="22" t="s">
         <v>380</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="22" t="s">
         <v>149</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="16" t="s">
         <v>383</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="22" t="s">
         <v>145</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="16" t="s">
         <v>147</v>
       </c>
     </row>
@@ -4888,7 +4935,7 @@
       <c r="C11" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="23" t="s">
         <v>325</v>
       </c>
     </row>
@@ -4902,7 +4949,7 @@
       <c r="C12" t="s">
         <v>176</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="23" t="s">
         <v>199</v>
       </c>
     </row>
@@ -4916,7 +4963,7 @@
       <c r="C13" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="23" t="s">
         <v>324</v>
       </c>
     </row>
@@ -4930,7 +4977,7 @@
       <c r="C14" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="23" t="s">
         <v>178</v>
       </c>
     </row>
@@ -4944,7 +4991,7 @@
       <c r="C15" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="24" t="s">
         <v>343</v>
       </c>
     </row>
@@ -4958,7 +5005,7 @@
       <c r="C16" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="D16" s="24" t="s">
         <v>172</v>
       </c>
     </row>
@@ -4972,11 +5019,11 @@
       <c r="C17" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="D17" s="18" t="s">
+      <c r="D17" s="24" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>184</v>
       </c>
@@ -4990,7 +5037,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>185</v>
       </c>
@@ -5004,7 +5051,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>187</v>
       </c>
@@ -5018,7 +5065,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>189</v>
       </c>
@@ -5032,7 +5079,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>198</v>
       </c>
@@ -5046,7 +5093,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>181</v>
       </c>
@@ -5060,7 +5107,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>182</v>
       </c>
@@ -5074,7 +5121,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>183</v>
       </c>
@@ -5088,7 +5135,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="345" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="345" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>191</v>
       </c>
@@ -5102,7 +5149,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>192</v>
       </c>
@@ -5116,7 +5163,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>194</v>
       </c>
@@ -5130,7 +5177,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>94</v>
       </c>
@@ -5144,7 +5191,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>201</v>
       </c>
@@ -5158,7 +5205,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>203</v>
       </c>
@@ -5172,7 +5219,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>205</v>
       </c>
@@ -5186,7 +5233,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>206</v>
       </c>
@@ -5200,7 +5247,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>208</v>
       </c>
@@ -5214,7 +5261,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>210</v>
       </c>
@@ -5228,7 +5275,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>212</v>
       </c>
@@ -5242,7 +5289,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>214</v>
       </c>
@@ -5256,7 +5303,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>216</v>
       </c>
@@ -5270,7 +5317,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>218</v>
       </c>
@@ -5284,7 +5331,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>220</v>
       </c>
@@ -5298,7 +5345,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>221</v>
       </c>
@@ -5312,7 +5359,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>223</v>
       </c>
@@ -5326,7 +5373,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>95</v>
       </c>
@@ -5340,7 +5387,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>225</v>
       </c>
@@ -5354,7 +5401,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>227</v>
       </c>
@@ -5368,7 +5415,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
         <v>229</v>
       </c>
@@ -5382,7 +5429,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>230</v>
       </c>
@@ -5396,7 +5443,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="48" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>232</v>
       </c>
@@ -5410,7 +5457,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>234</v>
       </c>
@@ -5424,7 +5471,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>236</v>
       </c>
@@ -5438,7 +5485,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>237</v>
       </c>
@@ -5452,7 +5499,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>239</v>
       </c>
@@ -5466,7 +5513,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>241</v>
       </c>
@@ -5480,7 +5527,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>242</v>
       </c>
@@ -5494,7 +5541,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>243</v>
       </c>
@@ -5508,7 +5555,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>245</v>
       </c>
@@ -5522,7 +5569,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>96</v>
       </c>
@@ -5536,7 +5583,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>249</v>
       </c>
@@ -5550,7 +5597,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>251</v>
       </c>
@@ -5564,7 +5611,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>253</v>
       </c>
@@ -5578,7 +5625,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>254</v>
       </c>
@@ -5592,7 +5639,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>256</v>
       </c>
@@ -5606,7 +5653,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>258</v>
       </c>
@@ -5620,7 +5667,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>260</v>
       </c>
@@ -5634,7 +5681,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="65" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>262</v>
       </c>
@@ -5648,7 +5695,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="66" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>264</v>
       </c>
@@ -5662,7 +5709,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>266</v>
       </c>
@@ -5676,7 +5723,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>267</v>
       </c>
@@ -5690,7 +5737,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="69" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>268</v>
       </c>
@@ -5704,7 +5751,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="70" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>270</v>
       </c>
@@ -5718,7 +5765,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="71" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
         <v>97</v>
       </c>
@@ -5732,7 +5779,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="72" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
         <v>277</v>
       </c>
@@ -5746,7 +5793,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="73" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
         <v>279</v>
       </c>
@@ -5760,7 +5807,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="74" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
         <v>281</v>
       </c>
@@ -5774,7 +5821,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="75" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
         <v>282</v>
       </c>
@@ -5788,7 +5835,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="76" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>284</v>
       </c>
@@ -5802,7 +5849,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="77" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
         <v>286</v>
       </c>
@@ -5816,7 +5863,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="78" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>288</v>
       </c>
@@ -5830,7 +5877,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="79" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>289</v>
       </c>
@@ -5844,7 +5891,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="80" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>291</v>
       </c>
@@ -5858,7 +5905,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>293</v>
       </c>
@@ -5872,7 +5919,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>295</v>
       </c>
@@ -5886,7 +5933,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="83" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>296</v>
       </c>
@@ -5900,7 +5947,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>298</v>
       </c>
@@ -5914,7 +5961,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="85" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="14" t="s">
         <v>302</v>
       </c>
@@ -5928,7 +5975,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="86" spans="1:4" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="14" t="s">
         <v>313</v>
       </c>
@@ -5942,7 +5989,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" ht="150" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
         <v>304</v>
       </c>
@@ -5956,7 +6003,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="88" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
         <v>305</v>
       </c>
@@ -5970,7 +6017,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="89" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>306</v>
       </c>
@@ -5984,7 +6031,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="90" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
         <v>309</v>
       </c>
@@ -5998,7 +6045,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="91" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
         <v>311</v>
       </c>
@@ -6012,7 +6059,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="92" spans="1:4" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="14" t="s">
         <v>315</v>
       </c>
@@ -6026,7 +6073,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="330" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" ht="330" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>312</v>
       </c>
@@ -6040,7 +6087,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="94" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
         <v>296</v>
       </c>
@@ -6054,7 +6101,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="95" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
         <v>298</v>
       </c>
@@ -6068,7 +6115,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="96" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
         <v>317</v>
       </c>
@@ -6082,7 +6129,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="97" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>318</v>
       </c>
@@ -6096,7 +6143,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="98" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="14" t="s">
         <v>319</v>
       </c>
@@ -6110,7 +6157,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="330" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" ht="330" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
         <v>321</v>
       </c>
@@ -6124,7 +6171,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="100" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
         <v>296</v>
       </c>
@@ -6138,7 +6185,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="101" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
         <v>298</v>
       </c>
@@ -6153,28 +6200,24 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="22" t="s">
+      <c r="A102" s="19" t="s">
         <v>344</v>
       </c>
-      <c r="B102" s="23" t="s">
+      <c r="B102" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C102" s="22" t="s">
+      <c r="C102" s="19" t="s">
         <v>344</v>
       </c>
-      <c r="D102" s="15" t="s">
+      <c r="D102" s="23" t="s">
         <v>345</v>
       </c>
     </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D103" s="23"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:E102">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="All"/>
-        <filter val="Short Sale"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:E102"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="46" fitToHeight="0" orientation="landscape" horizontalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>